<commit_message>
add ptu and more msr
</commit_message>
<xml_diff>
--- a/svr_info/pcie/Result.xlsx
+++ b/svr_info/pcie/Result.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="PCIE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PCIE" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -355,7 +355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,16 +378,16 @@
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>00:13.0
- PCI bridge: Intel Corporation Device 1bb3 (rev 11) (prog-if 00 [Normal decode])
-Speed 5GT/s, Width x1</t>
+          <t>00:0d.0
+ PCI bridge: Intel Corporation Device 1bbd (rev 11) (prog-if 00 [Normal decode])
+no value</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>01:00.0
  PCI bridge: ASPEED Technology, Inc. AST1150 PCI-to-PCI Bridge (rev 06) (prog-if 00 [Normal decode])
-Speed 5GT/s, Width x1</t>
+no value</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -418,7 +418,7 @@
         <is>
           <t>01:00.0
  PCI bridge: ASPEED Technology, Inc. AST1150 PCI-to-PCI Bridge (rev 06) (prog-if 00 [Normal decode])
-Speed 5GT/s, Width x1</t>
+no value</t>
         </is>
       </c>
     </row>
@@ -439,7 +439,6 @@
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>38:00.0
- Non-Volatile memory controller: Intel Corporation Device 0b60 (prog-if 02 [NVM Express])
 no value</t>
         </is>
       </c>
@@ -453,15 +452,15 @@
     <row r="9">
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>37:03.0
- PCI bridge: Intel Corporation Device 352b (rev 04) (prog-if 00 [Normal decode])
+          <t>48:01.0
+ PCI bridge: Intel Corporation Device 352a (rev 04) (prog-if 00 [Normal decode])
 no value</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>39:00.0
- Non-Volatile memory controller: Intel Corporation Device 0b60 (prog-if 02 [NVM Express])
+          <t>49:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
 no value</t>
         </is>
       </c>
@@ -475,15 +474,15 @@
     <row r="11">
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>37:05.0
- PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
+          <t>48:03.0
+ PCI bridge: Intel Corporation Device 352b (rev 04) (prog-if 00 [Normal decode])
 no value</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>3a:00.0
- Non-Volatile memory controller: Intel Corporation Device 0b60 (prog-if 02 [NVM Express])
+          <t>4a:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
 no value</t>
         </is>
       </c>
@@ -497,15 +496,14 @@
     <row r="13">
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>37:07.0
- PCI bridge: Intel Corporation Device 352d (rev 04) (prog-if 00 [Normal decode])
+          <t>48:05.0
+ PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
 no value</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>3b:00.0
- Non-Volatile memory controller: Intel Corporation Device 0b60 (prog-if 02 [NVM Express])
+          <t>4b:00.0
 no value</t>
         </is>
       </c>
@@ -517,86 +515,306 @@
       <c r="D14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>59:01.0
+ PCI bridge: Intel Corporation Device 352a (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>5a:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>59:03.0
+ PCI bridge: Intel Corporation Device 352b (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>5b:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>59:05.0
+ PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>5c:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>59:07.0
+ PCI bridge: Intel Corporation Device 352d (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>5d:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>Socket 1</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>a7:01.0
+    <row r="24">
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>80:05.0
+ PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>81:00.0
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n"/>
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>80:07.0
+ PCI bridge: Intel Corporation Device 352d (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>82:00.0
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>97:01.0
  PCI bridge: Intel Corporation Device 352a (rev 04) (prog-if 00 [Normal decode])
-Speed 2.5GT/s, Width x0</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>a8:00.0
-no value</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>a7:03.0
+no value</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>98:00.0
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n"/>
+      <c r="B29" s="2" t="n"/>
+      <c r="C29" s="2" t="n"/>
+      <c r="D29" s="2" t="n"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>c7:01.0
+ PCI bridge: Intel Corporation Device 352a (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>c8:00.0
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n"/>
+      <c r="B31" s="2" t="n"/>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="2" t="n"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>c7:05.0
+ PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>c9:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n"/>
+      <c r="B33" s="2" t="n"/>
+      <c r="C33" s="2" t="n"/>
+      <c r="D33" s="2" t="n"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>c7:07.0
+ PCI bridge: Intel Corporation Device 352d (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>ca:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n"/>
+      <c r="B35" s="2" t="n"/>
+      <c r="C35" s="2" t="n"/>
+      <c r="D35" s="2" t="n"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>d7:01.0
+ PCI bridge: Intel Corporation Device 352a (rev 04) (prog-if 00 [Normal decode])
+no value</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>d8:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n"/>
+      <c r="B37" s="2" t="n"/>
+      <c r="C37" s="2" t="n"/>
+      <c r="D37" s="2" t="n"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>d7:03.0
  PCI bridge: Intel Corporation Device 352b (rev 04) (prog-if 00 [Normal decode])
-Speed 2.5GT/s, Width x0</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>a9:00.0
-no value</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>a7:05.0
+no value</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>d9:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n"/>
+      <c r="B39" s="2" t="n"/>
+      <c r="C39" s="2" t="n"/>
+      <c r="D39" s="2" t="n"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>d7:05.0
  PCI bridge: Intel Corporation Device 352c (rev 04) (prog-if 00 [Normal decode])
-Speed 2.5GT/s, Width x0</t>
-        </is>
-      </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>aa:00.0
-no value</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
-      <c r="C21" s="2" t="n"/>
-      <c r="D21" s="2" t="n"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>a7:07.0
+no value</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>da:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
+no value</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n"/>
+      <c r="B41" s="2" t="n"/>
+      <c r="C41" s="2" t="n"/>
+      <c r="D41" s="2" t="n"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>d7:07.0
  PCI bridge: Intel Corporation Device 352d (rev 04) (prog-if 00 [Normal decode])
-Speed 2.5GT/s, Width x0</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>ab:00.0
+no value</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>db:00.0
+ Non-Volatile memory controller: Intel Corporation NVMe DC SSD [3DNAND, Sentinel Rock Controller] (prog-if 02 [NVM Express])
 no value</t>
         </is>
       </c>

</xml_diff>